<commit_message>
fix: Various fixes; working on integrating meeting notes
</commit_message>
<xml_diff>
--- a/inst/template/template.xlsx
+++ b/inst/template/template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="STAT" sheetId="1" state="visible" r:id="rId2"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="140">
   <si>
     <t xml:space="preserve">User ID</t>
   </si>
@@ -508,6 +508,15 @@
   </si>
   <si>
     <t xml:space="preserve">Ions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pressure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Light</t>
   </si>
 </sst>
 </file>
@@ -610,7 +619,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -653,6 +662,12 @@
         <bgColor rgb="FF9DC3E6"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFBBE33D"/>
+        <bgColor rgb="FFC5E0B4"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
@@ -717,7 +732,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -775,6 +790,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -837,7 +856,7 @@
       <rgbColor rgb="FFFFCC99"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFBBE33D"/>
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
@@ -863,7 +882,7 @@
   </sheetPr>
   <dimension ref="A1:Z1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="H9" activeCellId="0" sqref="H9"/>
@@ -874,7 +893,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.45"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="3" style="1" width="11.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="9.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="9.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="16.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="10" style="1" width="5.89"/>
@@ -1266,9 +1285,9 @@
       <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.70703125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.12"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1338,13 +1357,13 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.70703125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="21.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="27.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="19.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="18.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="19.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="18.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="14.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="16"/>
   </cols>
@@ -1521,12 +1540,12 @@
       <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.70703125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="31.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="40.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="40.43"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="29.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1614,7 +1633,7 @@
       <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.70703125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.45"/>
@@ -1685,7 +1704,7 @@
       <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.70703125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.89"/>
   </cols>
@@ -1738,7 +1757,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.70703125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
@@ -1757,17 +1776,17 @@
   </sheetPr>
   <dimension ref="A1:I1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.70703125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="54.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="27.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="54.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="27.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="33.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="22.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="22.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="29.56"/>
   </cols>
   <sheetData>
@@ -2000,6 +2019,21 @@
       </c>
       <c r="I19" s="0" t="s">
         <v>125</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H20" s="15" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H21" s="15" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H22" s="15" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Fixes and features; gibhub pages
</commit_message>
<xml_diff>
--- a/inst/template/template.xlsx
+++ b/inst/template/template.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="148">
   <si>
     <t xml:space="preserve">User ID</t>
   </si>
@@ -282,6 +282,9 @@
   </si>
   <si>
     <t xml:space="preserve">Airtightness reference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Measurement location description</t>
   </si>
   <si>
     <t xml:space="preserve">Fresh air supply</t>
@@ -323,6 +326,9 @@
   </si>
   <si>
     <t xml:space="preserve">AMB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ambient</t>
   </si>
   <si>
     <t xml:space="preserve">Through occupant operated window only</t>
@@ -376,6 +382,9 @@
     <t xml:space="preserve">BED</t>
   </si>
   <si>
+    <t xml:space="preserve">Bedroom</t>
+  </si>
+  <si>
     <t xml:space="preserve">Through automatic operated window</t>
   </si>
   <si>
@@ -414,6 +423,9 @@
     <t xml:space="preserve">LIV</t>
   </si>
   <si>
+    <t xml:space="preserve">Living room</t>
+  </si>
+  <si>
     <t xml:space="preserve">Through permanent opening to the exterior (grille, …)</t>
   </si>
   <si>
@@ -429,6 +441,9 @@
     <t xml:space="preserve">BAT</t>
   </si>
   <si>
+    <t xml:space="preserve">Bathroom</t>
+  </si>
+  <si>
     <t xml:space="preserve">UFP</t>
   </si>
   <si>
@@ -441,6 +456,9 @@
     <t xml:space="preserve">KIT</t>
   </si>
   <si>
+    <t xml:space="preserve">Kitchen</t>
+  </si>
+  <si>
     <t xml:space="preserve">Through mechanically driven overflow (or recirculated air) from adjacent zones</t>
   </si>
   <si>
@@ -465,6 +483,9 @@
     <t xml:space="preserve">CCO</t>
   </si>
   <si>
+    <t xml:space="preserve">Central corridor</t>
+  </si>
+  <si>
     <t xml:space="preserve">PM10</t>
   </si>
   <si>
@@ -478,6 +499,9 @@
   </si>
   <si>
     <t xml:space="preserve">HOO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Home office</t>
   </si>
   <si>
     <t xml:space="preserve">NO2</t>
@@ -619,7 +643,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -664,6 +688,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFDBB6"/>
+        <bgColor rgb="FFFFF2CC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFBBE33D"/>
         <bgColor rgb="FFC5E0B4"/>
       </patternFill>
@@ -732,7 +762,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -793,7 +823,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="8" borderId="1" xfId="25" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -853,7 +887,7 @@
       <rgbColor rgb="FF9DC3E6"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FFFFDBB6"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FFBBE33D"/>
@@ -893,7 +927,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.45"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="3" style="1" width="11.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="9.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="9.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="16.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="10" style="1" width="5.89"/>
@@ -1285,7 +1319,7 @@
       <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.70703125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.72265625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.12"/>
   </cols>
@@ -1357,7 +1391,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.70703125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.72265625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="21.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.56"/>
@@ -1540,12 +1574,12 @@
       <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.70703125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.72265625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="31.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="40.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="40.42"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="29.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1604,7 +1638,7 @@
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C3" type="list">
-      <formula1>Definitions!$G$2:$G$8</formula1>
+      <formula1>Definitions!$H$2:$H$8</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E3" type="list">
@@ -1633,7 +1667,7 @@
       <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.70703125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.72265625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.45"/>
@@ -1679,7 +1713,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B3" type="list">
-      <formula1>Definitions!$H$2:$H$20</formula1>
+      <formula1>Definitions!$I$2:$I$20</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -1704,7 +1738,7 @@
       <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.70703125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.72265625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.89"/>
   </cols>
@@ -1757,7 +1791,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.70703125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.72265625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
@@ -1774,23 +1808,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I1048576"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
+      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.70703125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.72265625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="54.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="27.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="33.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="22.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="29.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="25.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="29.56"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="30.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2"/>
       <c r="B1" s="2" t="s">
         <v>82</v>
@@ -1804,239 +1839,271 @@
       <c r="E1" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="15" t="s">
         <v>85</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I1" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>94</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>102</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>62</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>109</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
         <v>58</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="G5" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="H5" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="H5" s="0" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I5" s="0" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="0" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>120</v>
+      </c>
+      <c r="I6" s="0" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="0" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>118</v>
+        <v>30</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>124</v>
+      </c>
+      <c r="I7" s="0" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C8" s="0" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>121</v>
-      </c>
-      <c r="H8" s="0" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>127</v>
+      </c>
+      <c r="G8" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="I8" s="0" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F9" s="0" t="s">
-        <v>123</v>
-      </c>
-      <c r="H9" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="G9" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="I9" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="J9" s="0" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F10" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="G10" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="I10" s="0" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F11" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="G11" s="0" t="s">
         <v>124</v>
       </c>
-      <c r="I9" s="0" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F10" s="0" t="s">
-        <v>126</v>
-      </c>
-      <c r="H10" s="0" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F11" s="0" t="s">
-        <v>128</v>
-      </c>
-      <c r="H11" s="0" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H12" s="0" t="s">
-        <v>130</v>
-      </c>
+      <c r="I11" s="0" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I12" s="0" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H13" s="0" t="s">
-        <v>131</v>
-      </c>
+        <v>138</v>
+      </c>
+      <c r="J12" s="0" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I13" s="0" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H14" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="J13" s="0" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H15" s="0" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H16" s="0" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H17" s="0" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H18" s="0" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H19" s="0" t="s">
-        <v>118</v>
-      </c>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I14" s="0" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I15" s="0" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I16" s="0" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I17" s="0" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I18" s="0" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I19" s="0" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H20" s="15" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H21" s="15" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H22" s="15" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>124</v>
+      </c>
+      <c r="J19" s="0" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I20" s="16" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I21" s="16" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I22" s="16" t="s">
+        <v>147</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
fix: Adding first draft of annex_write
</commit_message>
<xml_diff>
--- a/inst/template/template.xlsx
+++ b/inst/template/template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="STAT" sheetId="1" state="visible" r:id="rId2"/>
@@ -27,87 +27,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="148">
-  <si>
-    <t xml:space="preserve">User ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Study ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Home ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Room ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pollutant ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Period ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Time ID</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="124">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
   <si>
-    <t xml:space="preserve">Commit ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Avg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Std</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P2.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P25</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P50</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P75</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P97.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">eCDF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Start</t>
-  </si>
-  <si>
-    <t xml:space="preserve">End</t>
-  </si>
-  <si>
-    <t xml:space="preserve"># Samples</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Typ. SI (Sample intervall)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">% with Typ. SI</t>
-  </si>
-  <si>
-    <t xml:space="preserve"># NA's</t>
-  </si>
-  <si>
-    <t xml:space="preserve">% excluded</t>
-  </si>
-  <si>
-    <t xml:space="preserve">% Min cut</t>
-  </si>
-  <si>
-    <t xml:space="preserve">% Max cut</t>
-  </si>
-  <si>
     <t xml:space="preserve">Contact</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ORCID</t>
   </si>
   <si>
     <t xml:space="preserve">Year(s)</t>
@@ -643,7 +571,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -653,24 +581,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFF2CC"/>
-        <bgColor rgb="FFF2F2F2"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFE2F0D9"/>
-        <bgColor rgb="FFF2F2F2"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC5E0B4"/>
-        <bgColor rgb="FFE2F0D9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
         <bgColor rgb="FFE2F0D9"/>
       </patternFill>
     </fill>
@@ -678,6 +588,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF9DC3E6"/>
         <bgColor rgb="FF8FAADC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE2F0D9"/>
+        <bgColor rgb="FFFFF2CC"/>
       </patternFill>
     </fill>
     <fill>
@@ -695,7 +611,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFBBE33D"/>
-        <bgColor rgb="FFC5E0B4"/>
+        <bgColor rgb="FFFFCC00"/>
       </patternFill>
     </fill>
   </fills>
@@ -762,7 +678,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -771,6 +687,10 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="25" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="8" fillId="2" borderId="1" xfId="25" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -783,51 +703,59 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="5" borderId="1" xfId="25" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="25" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="1" xfId="25" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="6" borderId="1" xfId="25" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="8" borderId="1" xfId="25" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -849,7 +777,7 @@
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFF2F2F2"/>
+      <rgbColor rgb="FFFFFFFF"/>
       <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
@@ -871,7 +799,7 @@
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0563C1"/>
-      <rgbColor rgb="FFC5E0B4"/>
+      <rgbColor rgb="FFCCCCFF"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -914,12 +842,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z1048576"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="H9" activeCellId="0" sqref="H9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.4609375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -937,86 +863,8 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="28" style="1" width="11.45"/>
   </cols>
   <sheetData>
-    <row r="1" s="6" customFormat="true" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="U1" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="V1" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="W1" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="X1" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y1" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="Z1" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
+    <row r="1" s="2" customFormat="true" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048296" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048297" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048298" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048299" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1313,62 +1161,69 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F1048576"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.72265625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.78515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="43.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="25.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="32.13"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="8"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-    </row>
-    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="C3" s="9" t="n">
+      <c r="B3" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7" t="n">
         <v>2012</v>
       </c>
-      <c r="D3" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-    </row>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="E3" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
@@ -1387,127 +1242,131 @@
   </sheetPr>
   <dimension ref="A1:Q1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.72265625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.78515625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="21.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="27.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="19.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="18.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="14.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="32.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="32.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="0" width="13.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="11" style="0" width="32.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="13.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="14" style="0" width="32.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="13.02"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="63" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>49</v>
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="8"/>
-      <c r="B2" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="J2" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="K2" s="11"/>
-      <c r="L2" s="8"/>
-      <c r="M2" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="N2" s="8"/>
-      <c r="O2" s="8"/>
-      <c r="P2" s="8"/>
-      <c r="Q2" s="8"/>
+      <c r="A2" s="6"/>
+      <c r="B2" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="K2" s="9"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="N2" s="6"/>
+      <c r="O2" s="6"/>
+      <c r="P2" s="6"/>
+      <c r="Q2" s="6"/>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="F3" s="13" t="n">
+        <v>31</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F3" s="11" t="n">
         <v>25</v>
       </c>
-      <c r="G3" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="H3" s="9" t="s">
-        <v>30</v>
+      <c r="G3" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>6</v>
       </c>
       <c r="I3" s="1" t="n">
         <v>0.6</v>
@@ -1515,23 +1374,23 @@
       <c r="J3" s="1" t="n">
         <v>50</v>
       </c>
-      <c r="K3" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="L3" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="M3" s="13" t="n">
+      <c r="K3" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="L3" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="M3" s="11" t="n">
         <v>70</v>
       </c>
-      <c r="N3" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="O3" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="P3" s="12" t="s">
-        <v>65</v>
+      <c r="N3" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="O3" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="P3" s="10" t="s">
+        <v>41</v>
       </c>
       <c r="Q3" s="0" t="n">
         <v>2008</v>
@@ -1570,65 +1429,66 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="102" zoomScaleNormal="102" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.72265625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.78515625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="31.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="40.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="49.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="60.26"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="29.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>69</v>
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="8"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="D3" s="13" t="n">
+        <v>46</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3" s="11" t="n">
         <v>10</v>
       </c>
-      <c r="E3" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="F3" s="9"/>
+      <c r="E3" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" s="7"/>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
@@ -1661,55 +1521,55 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E1048576"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.72265625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.78515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="31.26"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="10.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="33.52"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="29.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="8"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-    </row>
-    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="24.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="B3" s="14" t="s">
-        <v>78</v>
+        <v>53</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>54</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>55</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
     <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B3" type="list">
@@ -1732,43 +1592,40 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F1048576"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.72265625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.78515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="15" width="38.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1022" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-    </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="8"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-    </row>
-    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="6"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>57</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
@@ -1787,11 +1644,11 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.72265625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.78515625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
@@ -1810,11 +1667,11 @@
   </sheetPr>
   <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.72265625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.78515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="54.98"/>
@@ -1826,282 +1683,282 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="30.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2"/>
-      <c r="B1" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="F1" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="G1" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>87</v>
+      <c r="A1" s="3"/>
+      <c r="B1" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="0" t="s">
-        <v>88</v>
+        <v>64</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>89</v>
+        <v>65</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>90</v>
+        <v>66</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>91</v>
+        <v>67</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>92</v>
+        <v>68</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>93</v>
+        <v>69</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>94</v>
+        <v>70</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>95</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>96</v>
+        <v>72</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>97</v>
+        <v>73</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>98</v>
+        <v>74</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>99</v>
+        <v>75</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>100</v>
+        <v>76</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>101</v>
+        <v>77</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>102</v>
+        <v>78</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>103</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>105</v>
+        <v>81</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>62</v>
+        <v>38</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>106</v>
+        <v>82</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>107</v>
+        <v>83</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>108</v>
+        <v>84</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>109</v>
+        <v>85</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>110</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
-        <v>58</v>
+        <v>34</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>111</v>
+        <v>87</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>112</v>
+        <v>88</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>113</v>
+        <v>89</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>114</v>
+        <v>90</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>72</v>
+        <v>48</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>115</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="0" t="s">
-        <v>116</v>
+        <v>92</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>117</v>
+        <v>93</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>118</v>
+        <v>94</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>119</v>
+        <v>95</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>120</v>
+        <v>96</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>121</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="0" t="s">
-        <v>122</v>
+        <v>98</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>123</v>
+        <v>99</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>124</v>
+        <v>100</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>125</v>
+        <v>101</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C8" s="0" t="s">
-        <v>126</v>
+        <v>102</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>127</v>
+        <v>103</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>128</v>
+        <v>104</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>129</v>
+        <v>105</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F9" s="0" t="s">
-        <v>130</v>
+        <v>106</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>131</v>
+        <v>107</v>
       </c>
       <c r="J9" s="0" t="s">
-        <v>132</v>
+        <v>108</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F10" s="0" t="s">
-        <v>133</v>
+        <v>109</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>134</v>
+        <v>110</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>135</v>
+        <v>111</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F11" s="0" t="s">
-        <v>136</v>
+        <v>112</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>124</v>
+        <v>100</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>137</v>
+        <v>113</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I12" s="0" t="s">
-        <v>138</v>
+        <v>114</v>
       </c>
       <c r="J12" s="0" t="s">
-        <v>132</v>
+        <v>108</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I13" s="0" t="s">
-        <v>139</v>
+        <v>115</v>
       </c>
       <c r="J13" s="0" t="s">
-        <v>132</v>
+        <v>108</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I14" s="0" t="s">
-        <v>140</v>
+        <v>116</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I15" s="0" t="s">
-        <v>141</v>
+        <v>117</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I16" s="0" t="s">
-        <v>142</v>
+        <v>118</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I17" s="0" t="s">
-        <v>143</v>
+        <v>119</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I18" s="0" t="s">
-        <v>144</v>
+        <v>120</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I19" s="0" t="s">
-        <v>124</v>
+        <v>100</v>
       </c>
       <c r="J19" s="0" t="s">
-        <v>132</v>
+        <v>108</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I20" s="16" t="s">
-        <v>145</v>
+      <c r="I20" s="19" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I21" s="16" t="s">
-        <v>146</v>
+      <c r="I21" s="19" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I22" s="16" t="s">
-        <v>147</v>
+      <c r="I22" s="19" t="s">
+        <v>123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: Silencing call in vignette; changed default sheet in template
</commit_message>
<xml_diff>
--- a/inst/template/template.xlsx
+++ b/inst/template/template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="STAT" sheetId="1" state="visible" r:id="rId2"/>
@@ -27,7 +27,31 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="132">
+  <si>
+    <t xml:space="preserve">NOTE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Filled</t>
+  </si>
+  <si>
+    <t xml:space="preserve">automatically</t>
+  </si>
+  <si>
+    <t xml:space="preserve">by</t>
+  </si>
+  <si>
+    <t xml:space="preserve">annex_write</t>
+  </si>
+  <si>
+    <t xml:space="preserve">don’t</t>
+  </si>
+  <si>
+    <t xml:space="preserve">manipulate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the data in here</t>
+  </si>
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -687,7 +711,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="25" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="25" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -842,10 +866,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:H1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.4609375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -863,7 +887,32 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="28" style="1" width="11.45"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="true" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1" s="2" customFormat="true" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
     <row r="1048296" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048297" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048298" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1167,7 +1216,7 @@
       <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.78515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="43.78"/>
@@ -1177,25 +1226,25 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1209,17 +1258,17 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="7" t="n">
         <v>2012</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
@@ -1246,11 +1295,11 @@
       <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.78515625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.93"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="32.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="32.99"/>
@@ -1263,80 +1312,80 @@
   <sheetData>
     <row r="1" customFormat="false" ht="63" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="N1" s="5" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="O1" s="5" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="P1" s="5" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="Q1" s="5" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6"/>
       <c r="B2" s="8" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
       <c r="F2" s="9" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="G2" s="6"/>
       <c r="H2" s="6"/>
       <c r="I2" s="9" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="J2" s="9" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="K2" s="9"/>
       <c r="L2" s="6"/>
       <c r="M2" s="9" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="N2" s="6"/>
       <c r="O2" s="6"/>
@@ -1345,28 +1394,28 @@
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="F3" s="11" t="n">
         <v>25</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="I3" s="1" t="n">
         <v>0.6</v>
@@ -1375,22 +1424,22 @@
         <v>50</v>
       </c>
       <c r="K3" s="7" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="L3" s="10" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="M3" s="11" t="n">
         <v>70</v>
       </c>
       <c r="N3" s="10" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="O3" s="10" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="P3" s="10" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="Q3" s="0" t="n">
         <v>2008</v>
@@ -1433,7 +1482,7 @@
       <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.78515625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.27"/>
@@ -1444,22 +1493,22 @@
   <sheetData>
     <row r="1" customFormat="false" ht="29.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1467,26 +1516,26 @@
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
       <c r="D2" s="9" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="D3" s="11" t="n">
         <v>10</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="F3" s="7"/>
     </row>
@@ -1527,29 +1576,29 @@
       <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.78515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="31.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="31.27"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="10.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="33.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="24.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1561,13 +1610,13 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1594,26 +1643,26 @@
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.78515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="15" width="38.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="15" width="38.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1022" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1623,7 +1672,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1648,7 +1697,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.78515625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
@@ -1671,7 +1720,7 @@
       <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.78515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="54.98"/>
@@ -1685,280 +1734,280 @@
     <row r="1" customFormat="false" ht="30.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="3"/>
       <c r="B1" s="3" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="F1" s="18" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="G1" s="18" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="0" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="0" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="0" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C8" s="0" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F9" s="0" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="J9" s="0" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F10" s="0" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F11" s="0" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I12" s="0" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="J12" s="0" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I13" s="0" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
       <c r="J13" s="0" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I14" s="0" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I15" s="0" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I16" s="0" t="s">
-        <v>118</v>
+        <v>126</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I17" s="0" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I18" s="0" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I19" s="0" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="J19" s="0" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I20" s="19" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I21" s="19" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I22" s="19" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix/feat: Implementing some of the changes suggested by GR via github
</commit_message>
<xml_diff>
--- a/inst/template/template.xlsx
+++ b/inst/template/template.xlsx
@@ -13,8 +13,8 @@
     <sheet name="META-Study" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="META-Home" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="META-Room" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="META-Pollutant" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="META-Period" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="META-Variable" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="META-Season" sheetId="7" state="visible" r:id="rId8"/>
     <sheet name="META-Time" sheetId="8" state="visible" r:id="rId9"/>
     <sheet name="Definitions" sheetId="9" state="visible" r:id="rId10"/>
   </sheets>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="143">
   <si>
     <t xml:space="preserve">IEA EBC Annex86 Dataset</t>
   </si>
@@ -237,13 +237,13 @@
     <t xml:space="preserve">Through mechanically driven supply air (no recirculated air)</t>
   </si>
   <si>
-    <t xml:space="preserve">Pollutant Name</t>
+    <t xml:space="preserve">Variable Name</t>
   </si>
   <si>
-    <t xml:space="preserve">Pollutant unit</t>
+    <t xml:space="preserve">Variable unit</t>
   </si>
   <si>
-    <t xml:space="preserve">Pollutant: add. Info</t>
+    <t xml:space="preserve">Variable: additional Info</t>
   </si>
   <si>
     <t xml:space="preserve">Measurement device</t>
@@ -252,7 +252,7 @@
     <t xml:space="preserve">GR-01-01-BR-CO2</t>
   </si>
   <si>
-    <t xml:space="preserve">PM other (add. info reqd)</t>
+    <t xml:space="preserve">PMOther</t>
   </si>
   <si>
     <t xml:space="preserve">ppm</t>
@@ -482,9 +482,6 @@
   </si>
   <si>
     <t xml:space="preserve">EHA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PMOther</t>
   </si>
   <si>
     <t xml:space="preserve">HOO</t>
@@ -976,9 +973,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>2102760</xdr:colOff>
+      <xdr:colOff>2101680</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>159480</xdr:rowOff>
+      <xdr:rowOff>158400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -992,7 +989,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="274320" y="305280"/>
-          <a:ext cx="1828440" cy="2292480"/>
+          <a:ext cx="1827360" cy="2291400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1015,13 +1012,13 @@
   <dimension ref="B3:K38"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="71.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="71.3"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1167,7 +1164,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="10"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="3" width="10.42"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="3" style="3" width="11.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="3" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="3" width="9.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="8" style="3" width="9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="3" width="15.71"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="28" style="3" width="11.42"/>
@@ -1206,9 +1203,9 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="43.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="25.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="32.15"/>
@@ -1277,19 +1274,19 @@
       <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="0" width="13.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="0" width="13.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="11" style="0" width="33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="13.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="13.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="14" style="0" width="33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="24.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="24.41"/>
   </cols>
   <sheetData>
     <row r="1" s="17" customFormat="true" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -19758,7 +19755,7 @@
       <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.28"/>
@@ -27825,10 +27822,10 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="31.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="15.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="33.57"/>
   </cols>
@@ -31881,9 +31878,9 @@
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="23" width="38.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1022" style="0" width="11.57"/>
   </cols>
@@ -31926,7 +31923,7 @@
       <selection pane="topLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
@@ -31949,10 +31946,10 @@
       <selection pane="topLeft" activeCell="I20" activeCellId="0" sqref="I20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="54.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="54.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="27.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="33.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.28"/>
@@ -32180,7 +32177,7 @@
         <v>56</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>128</v>
+        <v>74</v>
       </c>
       <c r="J9" s="24" t="n">
         <f aca="false">TRUE()</f>
@@ -32189,13 +32186,13 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F10" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="G10" s="0" t="s">
         <v>129</v>
       </c>
-      <c r="G10" s="0" t="s">
+      <c r="I10" s="0" t="s">
         <v>130</v>
-      </c>
-      <c r="I10" s="0" t="s">
-        <v>131</v>
       </c>
       <c r="J10" s="24" t="n">
         <f aca="false">FALSE()</f>
@@ -32204,13 +32201,13 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F11" s="0" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G11" s="0" t="s">
         <v>121</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J11" s="24" t="n">
         <f aca="false">FALSE()</f>
@@ -32219,7 +32216,7 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I12" s="0" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J12" s="24" t="n">
         <f aca="false">TRUE()</f>
@@ -32228,7 +32225,7 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I13" s="0" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J13" s="24" t="n">
         <f aca="false">TRUE()</f>
@@ -32237,7 +32234,7 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I14" s="0" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J14" s="24" t="n">
         <f aca="false">FALSE()</f>
@@ -32246,7 +32243,7 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I15" s="0" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J15" s="24" t="n">
         <f aca="false">FALSE()</f>
@@ -32255,7 +32252,7 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I16" s="0" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="J16" s="24" t="n">
         <f aca="false">FALSE()</f>
@@ -32264,7 +32261,7 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I17" s="0" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="J17" s="24" t="n">
         <f aca="false">FALSE()</f>
@@ -32273,7 +32270,7 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I18" s="0" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="J18" s="24" t="n">
         <f aca="false">FALSE()</f>
@@ -32291,7 +32288,7 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I20" s="25" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J20" s="24" t="n">
         <f aca="false">FALSE()</f>
@@ -32300,7 +32297,7 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I21" s="25" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="J21" s="24" t="n">
         <f aca="false">FALSE()</f>
@@ -32309,7 +32306,7 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I22" s="25" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="J22" s="24" t="n">
         <f aca="false">FALSE()</f>

</xml_diff>

<commit_message>
fix: Trying to implement a series of changes discus in todays annex global meeting
</commit_message>
<xml_diff>
--- a/inst/template/template.xlsx
+++ b/inst/template/template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="INFO" sheetId="1" state="visible" r:id="rId2"/>
@@ -14,9 +14,7 @@
     <sheet name="META-Home" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="META-Room" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="META-Variable" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="META-Season" sheetId="7" state="visible" r:id="rId8"/>
-    <sheet name="META-Time" sheetId="8" state="visible" r:id="rId9"/>
-    <sheet name="Definitions" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="Definitions" sheetId="7" state="visible" r:id="rId8"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -28,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="143">
   <si>
     <t xml:space="preserve">IEA EBC Annex86 Dataset</t>
   </si>
@@ -258,12 +256,6 @@
     <t xml:space="preserve">ppm</t>
   </si>
   <si>
-    <t xml:space="preserve">Definition</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GR-01-01-BR-CO2-All</t>
-  </si>
-  <si>
     <t xml:space="preserve">Vent type</t>
   </si>
   <si>
@@ -283,6 +275,12 @@
   </si>
   <si>
     <t xml:space="preserve">Pollution: Additional information required</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lower bound</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Upper bound</t>
   </si>
   <si>
     <t xml:space="preserve">Window airing (not designed)</t>
@@ -779,7 +777,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -870,10 +868,6 @@
     </xf>
     <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -973,9 +967,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>2101680</xdr:colOff>
+      <xdr:colOff>2100960</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>158400</xdr:rowOff>
+      <xdr:rowOff>157680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -989,7 +983,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="274320" y="305280"/>
-          <a:ext cx="1827360" cy="2291400"/>
+          <a:ext cx="1826640" cy="2290680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1011,11 +1005,11 @@
   </sheetPr>
   <dimension ref="B3:K38"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="71.3"/>
@@ -1141,8 +1135,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Standard"&amp;12&amp;Kffffff&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12&amp;KffffffSeite &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffSeite &amp;P</oddFooter>
   </headerFooter>
   <drawing r:id="rId2"/>
 </worksheet>
@@ -1203,7 +1197,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.95703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="43.71"/>
@@ -1274,7 +1268,7 @@
       <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.95703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.02"/>
@@ -19752,10 +19746,10 @@
   <dimension ref="A1:F1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.95703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.28"/>
@@ -19768,7 +19762,7 @@
       <c r="A1" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="16" t="s">
         <v>62</v>
       </c>
       <c r="C1" s="16" t="s">
@@ -27822,7 +27816,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.95703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.4"/>
@@ -31872,81 +31866,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L4" activeCellId="0" sqref="L4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="23" width="38.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1022" style="0" width="11.57"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="C1" s="15" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>77</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="10.921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:J22"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I20" activeCellId="0" sqref="I20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="10.921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.95703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="54.98"/>
@@ -31962,30 +31888,36 @@
     <row r="1" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="13"/>
       <c r="B1" s="15" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D1" s="16" t="s">
         <v>44</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F1" s="16" t="s">
         <v>62</v>
       </c>
       <c r="G1" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="H1" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="I1" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="J1" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="I1" s="16" t="s">
+      <c r="K1" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="J1" s="16" t="s">
+      <c r="L1" s="16" t="s">
         <v>84</v>
       </c>
     </row>
@@ -32014,12 +31946,18 @@
       <c r="I2" s="0" t="s">
         <v>92</v>
       </c>
-      <c r="J2" s="24" t="n">
+      <c r="J2" s="23" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L2" s="0" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
         <v>93</v>
       </c>
@@ -32044,12 +31982,18 @@
       <c r="I3" s="0" t="s">
         <v>100</v>
       </c>
-      <c r="J3" s="24" t="n">
+      <c r="J3" s="23" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3" s="0" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
         <v>101</v>
       </c>
@@ -32074,12 +32018,18 @@
       <c r="I4" s="0" t="s">
         <v>107</v>
       </c>
-      <c r="J4" s="24" t="n">
+      <c r="J4" s="23" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L4" s="0" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
         <v>53</v>
       </c>
@@ -32101,12 +32051,18 @@
       <c r="I5" s="0" t="s">
         <v>112</v>
       </c>
-      <c r="J5" s="24" t="n">
+      <c r="J5" s="23" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L5" s="0" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="0" t="s">
         <v>113</v>
       </c>
@@ -32125,12 +32081,18 @@
       <c r="I6" s="0" t="s">
         <v>118</v>
       </c>
-      <c r="J6" s="24" t="n">
+      <c r="J6" s="23" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L6" s="0" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="0" t="s">
         <v>119</v>
       </c>
@@ -32146,12 +32108,18 @@
       <c r="I7" s="0" t="s">
         <v>122</v>
       </c>
-      <c r="J7" s="24" t="n">
+      <c r="J7" s="23" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" s="0" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C8" s="0" t="s">
         <v>123</v>
       </c>
@@ -32164,12 +32132,18 @@
       <c r="I8" s="0" t="s">
         <v>126</v>
       </c>
-      <c r="J8" s="24" t="n">
+      <c r="J8" s="23" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L8" s="0" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F9" s="0" t="s">
         <v>127</v>
       </c>
@@ -32179,12 +32153,12 @@
       <c r="I9" s="0" t="s">
         <v>74</v>
       </c>
-      <c r="J9" s="24" t="n">
+      <c r="J9" s="23" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F10" s="0" t="s">
         <v>128</v>
       </c>
@@ -32194,12 +32168,18 @@
       <c r="I10" s="0" t="s">
         <v>130</v>
       </c>
-      <c r="J10" s="24" t="n">
+      <c r="J10" s="23" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L10" s="0" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F11" s="0" t="s">
         <v>131</v>
       </c>
@@ -32209,108 +32189,180 @@
       <c r="I11" s="0" t="s">
         <v>132</v>
       </c>
-      <c r="J11" s="24" t="n">
+      <c r="J11" s="23" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L11" s="0" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I12" s="0" t="s">
         <v>133</v>
       </c>
-      <c r="J12" s="24" t="n">
+      <c r="J12" s="23" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L12" s="0" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I13" s="0" t="s">
         <v>134</v>
       </c>
-      <c r="J13" s="24" t="n">
+      <c r="J13" s="23" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L13" s="0" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I14" s="0" t="s">
         <v>135</v>
       </c>
-      <c r="J14" s="24" t="n">
+      <c r="J14" s="23" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K14" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L14" s="0" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I15" s="0" t="s">
         <v>136</v>
       </c>
-      <c r="J15" s="24" t="n">
+      <c r="J15" s="23" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L15" s="0" t="n">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I16" s="0" t="s">
         <v>137</v>
       </c>
-      <c r="J16" s="24" t="n">
+      <c r="J16" s="23" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L16" s="0" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I17" s="0" t="s">
         <v>138</v>
       </c>
-      <c r="J17" s="24" t="n">
+      <c r="J17" s="23" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L17" s="0" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I18" s="0" t="s">
         <v>139</v>
       </c>
-      <c r="J18" s="24" t="n">
+      <c r="J18" s="23" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K18" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L18" s="0" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I19" s="0" t="s">
         <v>121</v>
       </c>
-      <c r="J19" s="24" t="n">
+      <c r="J19" s="23" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I20" s="25" t="s">
+      <c r="K19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L19" s="0" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I20" s="0" t="s">
         <v>140</v>
       </c>
-      <c r="J20" s="24" t="n">
+      <c r="J20" s="23" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
+      <c r="K20" s="0" t="n">
+        <v>-50</v>
+      </c>
+      <c r="L20" s="0" t="n">
+        <v>50</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I21" s="25" t="s">
+      <c r="I21" s="24" t="s">
         <v>141</v>
       </c>
-      <c r="J21" s="24" t="n">
+      <c r="J21" s="23" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
+      <c r="K21" s="0" t="n">
+        <v>500</v>
+      </c>
+      <c r="L21" s="0" t="n">
+        <v>1100</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I22" s="25" t="s">
+      <c r="I22" s="24" t="s">
         <v>142</v>
       </c>
-      <c r="J22" s="24" t="n">
+      <c r="J22" s="23" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
+      </c>
+      <c r="K22" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L22" s="0" t="n">
+        <v>5555</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: Pushing version 0.2-4 to the version 0.2 branch
</commit_message>
<xml_diff>
--- a/inst/template/template.xlsx
+++ b/inst/template/template.xlsx
@@ -1062,9 +1062,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>2094120</xdr:colOff>
+      <xdr:colOff>2093760</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>73080</xdr:rowOff>
+      <xdr:rowOff>72720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1078,7 +1078,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="274320" y="305280"/>
-          <a:ext cx="1819800" cy="2015640"/>
+          <a:ext cx="1819440" cy="2015280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1104,7 +1104,7 @@
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="71.3"/>
@@ -1310,7 +1310,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.2734375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.2890625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="19" width="18.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="43.71"/>
@@ -1383,7 +1383,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.2734375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.2890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.38"/>
@@ -19864,7 +19864,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.2734375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.2890625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="19" width="29.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33.14"/>
@@ -29937,7 +29937,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.2734375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.2890625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="19" width="31.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="19" width="26.63"/>
@@ -32995,7 +32995,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.2734375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.2890625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="54.98"/>
@@ -33086,7 +33086,7 @@
         <v>0</v>
       </c>
       <c r="M2" s="0" t="n">
-        <v>1000</v>
+        <v>2500</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
minor update template, occup type, bounds
</commit_message>
<xml_diff>
--- a/inst/template/template.xlsx
+++ b/inst/template/template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20394"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20395"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Daten\A86\R_DAP_git\annex\inst\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9AA193E1-201B-4EFC-ACDF-62C2A872FC05}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{824CBA63-42BA-4257-A866-8CBE6E1A24F4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="160">
   <si>
     <t>IEA EBC Annex86 Dataset</t>
   </si>
@@ -579,6 +579,9 @@
   <si>
     <t>Light</t>
   </si>
+  <si>
+    <t>unknown</t>
+  </si>
 </sst>
 </file>
 
@@ -600,7 +603,7 @@
       <sz val="11"/>
       <color rgb="FF0563C1"/>
       <name val="Arial"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
@@ -614,7 +617,7 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -20053,7 +20056,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:H1000"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -30116,14 +30121,11 @@
           </x14:formula2>
           <xm:sqref>G2:G1000</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0400-000002000000}">
+        <x14:dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" xr:uid="{7281A8AD-2F30-436E-82C4-A12F0F660B58}">
           <x14:formula1>
-            <xm:f>Definitions!$F$2:$F$6</xm:f>
+            <xm:f>Definitions!$F$2:$F$7</xm:f>
           </x14:formula1>
-          <x14:formula2>
-            <xm:f>0</xm:f>
-          </x14:formula2>
-          <xm:sqref>C2:C875</xm:sqref>
+          <xm:sqref>C2:C1000</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -30135,7 +30137,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AMJ1000"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -33183,7 +33187,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:N22"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="N13" sqref="N13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -33276,7 +33282,7 @@
         <v>0</v>
       </c>
       <c r="M2">
-        <v>2500</v>
+        <v>100000000</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -33315,7 +33321,7 @@
         <v>0</v>
       </c>
       <c r="M3">
-        <v>1000</v>
+        <v>100000000</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -33354,7 +33360,7 @@
         <v>0</v>
       </c>
       <c r="M4">
-        <v>500</v>
+        <v>100000000</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -33390,7 +33396,7 @@
         <v>0</v>
       </c>
       <c r="M5">
-        <v>500</v>
+        <v>100000000</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -33399,6 +33405,9 @@
       </c>
       <c r="D6" t="s">
         <v>124</v>
+      </c>
+      <c r="F6" t="s">
+        <v>159</v>
       </c>
       <c r="G6" t="s">
         <v>125</v>
@@ -33420,7 +33429,7 @@
         <v>0</v>
       </c>
       <c r="M6">
-        <v>500</v>
+        <v>100000000</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
@@ -33447,7 +33456,7 @@
         <v>0</v>
       </c>
       <c r="M7">
-        <v>500</v>
+        <v>100000000</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -33471,7 +33480,7 @@
         <v>0</v>
       </c>
       <c r="M8">
-        <v>500</v>
+        <v>100000000</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -33507,7 +33516,7 @@
         <v>0</v>
       </c>
       <c r="M10">
-        <v>500</v>
+        <v>100000000</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
@@ -33528,7 +33537,7 @@
         <v>0</v>
       </c>
       <c r="M11">
-        <v>500</v>
+        <v>100000000</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -33543,7 +33552,7 @@
         <v>0</v>
       </c>
       <c r="M12">
-        <v>500</v>
+        <v>100000000</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
@@ -33558,7 +33567,7 @@
         <v>0</v>
       </c>
       <c r="M13">
-        <v>500</v>
+        <v>100000000</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -33573,7 +33582,7 @@
         <v>0</v>
       </c>
       <c r="M14">
-        <v>500</v>
+        <v>100000000</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -33606,7 +33615,7 @@
         <v>0</v>
       </c>
       <c r="M16">
-        <v>500</v>
+        <v>100000000</v>
       </c>
     </row>
     <row r="17" spans="10:14" x14ac:dyDescent="0.25">
@@ -33621,7 +33630,7 @@
         <v>0</v>
       </c>
       <c r="M17">
-        <v>500</v>
+        <v>100000000</v>
       </c>
     </row>
     <row r="18" spans="10:14" x14ac:dyDescent="0.25">
@@ -33636,7 +33645,7 @@
         <v>0</v>
       </c>
       <c r="M18">
-        <v>500</v>
+        <v>100000000</v>
       </c>
     </row>
     <row r="19" spans="10:14" x14ac:dyDescent="0.25">
@@ -33651,7 +33660,7 @@
         <v>0</v>
       </c>
       <c r="M19">
-        <v>500</v>
+        <v>100000000</v>
       </c>
     </row>
     <row r="20" spans="10:14" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
feat: Updating to version 0.2-8; minor modification on template
</commit_message>
<xml_diff>
--- a/inst/template/template.xlsx
+++ b/inst/template/template.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="177">
   <si>
     <t xml:space="preserve">IEA EBC Annex86 Dataset</t>
   </si>
@@ -474,6 +474,9 @@
   </si>
   <si>
     <t xml:space="preserve">#/cm3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exhaust air</t>
   </si>
   <si>
     <t xml:space="preserve">Design values (from ventilation system design)</t>
@@ -1104,9 +1107,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>2092680</xdr:colOff>
+      <xdr:colOff>2092320</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>71640</xdr:rowOff>
+      <xdr:rowOff>71280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1120,7 +1123,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="274320" y="295920"/>
-          <a:ext cx="1818360" cy="1918800"/>
+          <a:ext cx="1818000" cy="1918440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1146,7 +1149,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.046875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.06640625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="71.33"/>
@@ -1351,7 +1354,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.37109375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.390625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="19" width="18.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="43.66"/>
@@ -1424,7 +1427,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.37109375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.390625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.44"/>
@@ -1545,18 +1548,18 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="3" s="25" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="4" s="25" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="5" s="25" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="6" s="25" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="7" s="25" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="8" s="25" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="9" s="25" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="10" s="25" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="11" s="25" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="12" s="25" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="13" s="25" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="14" s="25" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="3" s="25" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="4" s="25" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="5" s="25" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="6" s="25" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7" s="25" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8" s="25" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="9" s="25" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="10" s="25" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="11" s="25" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="12" s="25" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="13" s="25" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="14" s="25" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="15" s="25" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="16" s="25" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="17" s="25" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -19880,7 +19883,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D2:D1000" type="list">
-      <formula1>Definitions!$B$2:$B$5</formula1>
+      <formula1>Definitions!$B$2:$B$6</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -19905,7 +19908,7 @@
       <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.37109375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.390625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="19" width="28.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33.11"/>
@@ -29978,7 +29981,7 @@
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.37109375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.390625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="19" width="31.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="19" width="26.56"/>
@@ -33030,11 +33033,11 @@
   </sheetPr>
   <dimension ref="A1:N23"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.37109375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.390625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="54.98"/>
@@ -33255,26 +33258,29 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C6" s="0" t="s">
+      <c r="B6" s="0" t="s">
         <v>126</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="C6" s="0" t="s">
         <v>127</v>
       </c>
-      <c r="F6" s="0" t="s">
+      <c r="D6" s="0" t="s">
         <v>128</v>
       </c>
-      <c r="G6" s="0" t="s">
+      <c r="F6" s="0" t="s">
         <v>129</v>
       </c>
-      <c r="H6" s="0" t="s">
+      <c r="G6" s="0" t="s">
         <v>130</v>
       </c>
-      <c r="I6" s="0" t="s">
+      <c r="H6" s="0" t="s">
         <v>131</v>
       </c>
+      <c r="I6" s="0" t="s">
+        <v>132</v>
+      </c>
       <c r="J6" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="K6" s="30" t="n">
         <f aca="false">FALSE()</f>
@@ -33287,24 +33293,24 @@
         <v>10000</v>
       </c>
       <c r="N6" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="J7" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="K7" s="30" t="n">
         <f aca="false">FALSE()</f>
@@ -33317,21 +33323,21 @@
         <v>10000</v>
       </c>
       <c r="N7" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C8" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="J8" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="K8" s="30" t="n">
         <f aca="false">FALSE()</f>
@@ -33344,18 +33350,18 @@
         <v>10000</v>
       </c>
       <c r="N8" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G9" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="J9" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="K9" s="30" t="n">
         <f aca="false">TRUE()</f>
@@ -33365,13 +33371,13 @@
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G10" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="J10" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="K10" s="30" t="n">
         <f aca="false">FALSE()</f>
@@ -33384,18 +33390,18 @@
         <v>10000</v>
       </c>
       <c r="N10" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G11" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="J11" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="K11" s="30" t="n">
         <f aca="false">FALSE()</f>
@@ -33408,18 +33414,18 @@
         <v>10000</v>
       </c>
       <c r="N11" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G12" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="J12" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="K12" s="30" t="n">
         <f aca="false">TRUE()</f>
@@ -33432,18 +33438,18 @@
         <v>10000</v>
       </c>
       <c r="N12" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G13" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="J13" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="K13" s="30" t="n">
         <f aca="false">TRUE()</f>
@@ -33456,18 +33462,18 @@
         <v>10000</v>
       </c>
       <c r="N13" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G14" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="J14" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="K14" s="30" t="n">
         <f aca="false">FALSE()</f>
@@ -33485,7 +33491,7 @@
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J15" s="0" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="K15" s="30" t="n">
         <f aca="false">FALSE()</f>
@@ -33498,12 +33504,12 @@
         <v>105</v>
       </c>
       <c r="N15" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J16" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="K16" s="30" t="n">
         <f aca="false">FALSE()</f>
@@ -33516,12 +33522,12 @@
         <v>10000</v>
       </c>
       <c r="N16" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J17" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="K17" s="30" t="n">
         <f aca="false">FALSE()</f>
@@ -33534,12 +33540,12 @@
         <v>1000000000</v>
       </c>
       <c r="N17" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J18" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="K18" s="30" t="n">
         <f aca="false">FALSE()</f>
@@ -33552,12 +33558,12 @@
         <v>1000000000</v>
       </c>
       <c r="N18" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J19" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="K19" s="30" t="n">
         <f aca="false">TRUE()</f>
@@ -33566,7 +33572,7 @@
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J20" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="K20" s="30" t="n">
         <f aca="false">FALSE()</f>
@@ -33579,12 +33585,12 @@
         <v>50</v>
       </c>
       <c r="N20" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J21" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="K21" s="30" t="n">
         <f aca="false">FALSE()</f>
@@ -33597,12 +33603,12 @@
         <v>1100</v>
       </c>
       <c r="N21" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J22" s="0" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="K22" s="30" t="n">
         <f aca="false">TRUE()</f>
@@ -33615,12 +33621,12 @@
         <v>1500</v>
       </c>
       <c r="N22" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J23" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="K23" s="30" t="n">
         <f aca="false">FALSE()</f>
@@ -33633,7 +33639,7 @@
         <v>500</v>
       </c>
       <c r="N23" s="0" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: Moving to 0.2-13, fixed a bug in annex_validate, checking Type of building in annex_validate (see News)
</commit_message>
<xml_diff>
--- a/inst/template/template.xlsx
+++ b/inst/template/template.xlsx
@@ -5,16 +5,16 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="INFO" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="STAT" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="META-Study" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="META-Home" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="META-Room" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="META-Variable" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="Definitions" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="INFO" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="STAT" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="META-Study" sheetId="3" state="visible" r:id="rId5"/>
+    <sheet name="META-Home" sheetId="4" state="visible" r:id="rId6"/>
+    <sheet name="META-Room" sheetId="5" state="visible" r:id="rId7"/>
+    <sheet name="META-Variable" sheetId="6" state="visible" r:id="rId8"/>
+    <sheet name="Definitions" sheetId="7" state="visible" r:id="rId9"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -202,7 +202,7 @@
     <t xml:space="preserve">Building volume specific [1/h]</t>
   </si>
   <si>
-    <t xml:space="preserve">Multi-family house (MFH)</t>
+    <t xml:space="preserve">Single family house (SFH)</t>
   </si>
   <si>
     <t xml:space="preserve">social housing</t>
@@ -305,9 +305,6 @@
   </si>
   <si>
     <t xml:space="preserve">Active tracer gas measurement (in context of study)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Single family house (SFH)</t>
   </si>
   <si>
     <r>
@@ -435,6 +432,9 @@
       </rPr>
       <t xml:space="preserve">low-hood / anemometer measurement (in context of study)</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Multi-family house (MFH)</t>
   </si>
   <si>
     <t xml:space="preserve">Floor area specific / [m³/hm²]:</t>
@@ -1108,9 +1108,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>2091240</xdr:colOff>
+      <xdr:colOff>2090520</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>70200</xdr:rowOff>
+      <xdr:rowOff>69480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1124,7 +1124,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="274320" y="295920"/>
-          <a:ext cx="1816920" cy="1917360"/>
+          <a:ext cx="1816200" cy="1916640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1139,6 +1139,112 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
@@ -1146,7 +1252,7 @@
   </sheetPr>
   <dimension ref="B3:K38"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1290,7 +1396,7 @@
   </sheetPr>
   <dimension ref="A1:U1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1351,7 +1457,7 @@
   </sheetPr>
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1424,7 +1530,7 @@
   </sheetPr>
   <dimension ref="A1:R1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1478,7 +1584,7 @@
       <c r="K1" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="L1" s="24" t="s">
+      <c r="L1" s="27" t="s">
         <v>44</v>
       </c>
       <c r="M1" s="24" t="s">
@@ -19991,13 +20097,17 @@
       <c r="Q1000" s="26"/>
     </row>
   </sheetData>
-  <dataValidations count="2">
+  <dataValidations count="3">
     <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="G2:G1000" type="list">
       <formula1>Definitions!$C$2:$C$8</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D2:D1000" type="list">
       <formula1>Definitions!$B$2:$B$6</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="L2:L1000" type="list">
+      <formula1>Definitions!$D$2:$D$6</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -20018,7 +20128,7 @@
   </sheetPr>
   <dimension ref="A1:H1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -30091,7 +30201,7 @@
   </sheetPr>
   <dimension ref="A1:E1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -33147,7 +33257,7 @@
   </sheetPr>
   <dimension ref="A1:N23"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -33214,25 +33324,25 @@
         <v>92</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>98</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>99</v>
       </c>
       <c r="K2" s="31" t="n">
         <f aca="false">FALSE()</f>
@@ -33245,36 +33355,36 @@
         <v>10000</v>
       </c>
       <c r="N2" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>108</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>109</v>
       </c>
       <c r="K3" s="31" t="n">
         <f aca="false">FALSE()</f>
@@ -33287,18 +33397,18 @@
         <v>100</v>
       </c>
       <c r="N3" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="1" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>112</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>58</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>113</v>
@@ -33329,7 +33439,7 @@
         <v>1000</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -33597,7 +33707,7 @@
         <v>100</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
fix: Type of building now handled as 'not mandatory' but keeps the XLSX data range
</commit_message>
<xml_diff>
--- a/inst/template/template.xlsx
+++ b/inst/template/template.xlsx
@@ -1108,9 +1108,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>2090520</xdr:colOff>
+      <xdr:colOff>2089800</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>69480</xdr:rowOff>
+      <xdr:rowOff>68760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1124,7 +1124,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="274320" y="295920"/>
-          <a:ext cx="1816200" cy="1916640"/>
+          <a:ext cx="1815480" cy="1915920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1584,7 +1584,7 @@
       <c r="K1" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="L1" s="27" t="s">
+      <c r="L1" s="24" t="s">
         <v>44</v>
       </c>
       <c r="M1" s="24" t="s">
@@ -20107,7 +20107,7 @@
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="L2:L1000" type="list">
-      <formula1>Definitions!$D$2:$D$6</formula1>
+      <formula1>Definitions!$D$2:$D$7</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
dev: Streamlining 'multiple occurences of a variable', not yet tested and the existing tests do complain once. Pre-alpha commit.
</commit_message>
<xml_diff>
--- a/inst/template/template.xlsx
+++ b/inst/template/template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="INFO" sheetId="1" state="visible" r:id="rId3"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="177">
   <si>
     <t xml:space="preserve">IEA EBC Annex86 Dataset</t>
   </si>
@@ -290,6 +290,9 @@
   </si>
   <si>
     <t xml:space="preserve">Additional information required</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Allowed</t>
   </si>
   <si>
     <t xml:space="preserve">Lower bound</t>
@@ -1108,9 +1111,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>2089800</xdr:colOff>
+      <xdr:colOff>2089080</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>68760</xdr:rowOff>
+      <xdr:rowOff>68040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1124,7 +1127,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="274320" y="295920"/>
-          <a:ext cx="1815480" cy="1915920"/>
+          <a:ext cx="1814760" cy="1915200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1252,7 +1255,7 @@
   </sheetPr>
   <dimension ref="B3:K38"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1530,7 +1533,7 @@
   </sheetPr>
   <dimension ref="A1:R1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -33255,13 +33258,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N23"/>
+  <dimension ref="A1:O23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.40625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.40625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="54.98"/>
@@ -33271,7 +33274,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="29.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="12.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="11" style="1" width="11.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -33315,131 +33318,143 @@
       <c r="N1" s="24" t="s">
         <v>90</v>
       </c>
+      <c r="O1" s="24" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>58</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="K2" s="31" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="L2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="M2" s="1" t="n">
         <v>350</v>
       </c>
-      <c r="M2" s="32" t="n">
+      <c r="N2" s="32" t="n">
         <v>10000</v>
       </c>
-      <c r="N2" s="1" t="s">
-        <v>99</v>
+      <c r="O2" s="1" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="K3" s="31" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="L3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="M3" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="M3" s="33" t="n">
+      <c r="N3" s="33" t="n">
         <v>100</v>
       </c>
-      <c r="N3" s="1" t="s">
-        <v>109</v>
+      <c r="O3" s="1" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="K4" s="31" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="L4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="M4" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="M4" s="33" t="n">
+      <c r="N4" s="33" t="n">
         <v>1000</v>
       </c>
-      <c r="N4" s="1" t="s">
-        <v>109</v>
+      <c r="O4" s="1" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -33447,420 +33462,477 @@
         <v>53</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>70</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="K5" s="31" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="L5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="M5" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="M5" s="33" t="n">
+      <c r="N5" s="33" t="n">
         <v>1000000000</v>
       </c>
-      <c r="N5" s="1" t="s">
-        <v>125</v>
+      <c r="O5" s="1" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="K6" s="31" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="L6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="M6" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="M6" s="33" t="n">
+      <c r="N6" s="33" t="n">
         <v>10000</v>
       </c>
-      <c r="N6" s="1" t="s">
-        <v>133</v>
+      <c r="O6" s="1" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="K7" s="31" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="L7" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="M7" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="M7" s="33" t="n">
+      <c r="N7" s="33" t="n">
         <v>10000</v>
       </c>
-      <c r="N7" s="1" t="s">
-        <v>133</v>
+      <c r="O7" s="1" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C8" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="K8" s="31" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="L8" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="M8" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="M8" s="33" t="n">
+      <c r="N8" s="33" t="n">
         <v>10000</v>
       </c>
-      <c r="N8" s="1" t="s">
-        <v>133</v>
+      <c r="O8" s="1" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G9" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="K9" s="31" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="M9" s="33"/>
+      <c r="L9" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="N9" s="33"/>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G10" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="K10" s="31" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="L10" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="M10" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="M10" s="33" t="n">
+      <c r="N10" s="33" t="n">
         <v>10000</v>
       </c>
-      <c r="N10" s="1" t="s">
-        <v>133</v>
+      <c r="O10" s="1" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G11" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="K11" s="31" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="L11" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="M11" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="M11" s="33" t="n">
+      <c r="N11" s="33" t="n">
         <v>10000</v>
       </c>
-      <c r="N11" s="1" t="s">
-        <v>133</v>
+      <c r="O11" s="1" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G12" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="K12" s="31" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="L12" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="M12" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="M12" s="33" t="n">
+      <c r="N12" s="33" t="n">
         <v>10000</v>
       </c>
-      <c r="N12" s="1" t="s">
-        <v>133</v>
+      <c r="O12" s="1" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G13" s="1" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="K13" s="31" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="L13" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="M13" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="M13" s="33" t="n">
+      <c r="N13" s="33" t="n">
         <v>10000</v>
       </c>
-      <c r="N13" s="1" t="s">
-        <v>133</v>
+      <c r="O13" s="1" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G14" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="K14" s="31" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="L14" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="M14" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="M14" s="33" t="n">
+      <c r="N14" s="33" t="n">
         <v>100</v>
       </c>
-      <c r="N14" s="1" t="s">
-        <v>109</v>
+      <c r="O14" s="1" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J15" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="K15" s="31" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="L15" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="M15" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="M15" s="1" t="n">
+      <c r="N15" s="1" t="n">
         <v>105</v>
       </c>
-      <c r="N15" s="1" t="s">
-        <v>161</v>
+      <c r="O15" s="1" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J16" s="1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="K16" s="31" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="L16" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="M16" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="M16" s="33" t="n">
+      <c r="N16" s="33" t="n">
         <v>10000</v>
       </c>
-      <c r="N16" s="1" t="s">
-        <v>163</v>
+      <c r="O16" s="1" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J17" s="1" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="K17" s="31" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="L17" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="M17" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="M17" s="33" t="n">
+      <c r="N17" s="33" t="n">
         <v>1000000000</v>
       </c>
-      <c r="N17" s="1" t="s">
-        <v>165</v>
+      <c r="O17" s="1" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J18" s="1" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="K18" s="31" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="L18" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="M18" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="M18" s="33" t="n">
+      <c r="N18" s="33" t="n">
         <v>1000000000</v>
       </c>
-      <c r="N18" s="1" t="s">
-        <v>167</v>
+      <c r="O18" s="1" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J19" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="K19" s="31" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
+      <c r="L19" s="1" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J20" s="1" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="K20" s="31" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="L20" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="M20" s="1" t="n">
         <v>-50</v>
       </c>
-      <c r="M20" s="1" t="n">
+      <c r="N20" s="1" t="n">
         <v>50</v>
       </c>
-      <c r="N20" s="1" t="s">
-        <v>169</v>
+      <c r="O20" s="1" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J21" s="1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="K21" s="31" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="L21" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="M21" s="1" t="n">
         <v>500</v>
       </c>
-      <c r="M21" s="1" t="n">
+      <c r="N21" s="1" t="n">
         <v>1100</v>
       </c>
-      <c r="N21" s="1" t="s">
-        <v>171</v>
+      <c r="O21" s="1" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J22" s="1" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="K22" s="31" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="L22" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="M22" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="M22" s="1" t="n">
+      <c r="N22" s="1" t="n">
         <v>1500</v>
       </c>
-      <c r="N22" s="1" t="s">
-        <v>173</v>
+      <c r="O22" s="1" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J23" s="1" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="K23" s="31" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="L23" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="M23" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="M23" s="1" t="n">
+      <c r="N23" s="1" t="n">
         <v>500</v>
       </c>
-      <c r="N23" s="1" t="s">
-        <v>175</v>
+      <c r="O23" s="1" t="s">
+        <v>176</v>
       </c>
     </row>
   </sheetData>
@@ -33884,6 +33956,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L2:L23" type="list">
+      <formula1>"1,10,100"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>